<commit_message>
Attempt to fix Day 9 part 2 (not successful)
</commit_message>
<xml_diff>
--- a/Day 9 - Rope bridge/spreadsheet.xlsx
+++ b/Day 9 - Rope bridge/spreadsheet.xlsx
@@ -1,32 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry Lang\Documents\GitHub\Advent-of-Code-2022\Day 9 - Rope bridge WIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80425c2a0d069ab9/Documents/GitHub/Advent-of-Code-2022/Day 9 - Rope bridge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B12CF5-661F-473E-A950-D25737082268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{65B12CF5-661F-473E-A950-D25737082268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D029AF3C-D61F-4116-8FE7-2E8E5C698AAF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>T</t>
   </si>
@@ -68,6 +81,30 @@
   </si>
   <si>
     <t>do not move</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>[[[0, 0], [0, 1], [0, 2], [0, 3]], [[0, 0], [0, 0], [0, 1], [0, 2]], [[0, 0], [0, 0], [0, 0], [0, 1]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]]]</t>
+  </si>
+  <si>
+    <t>[[[0, 0], [0, 1], [0, 2], [0, 3]], [[0, 0], [0, 0], [0, 1], [0, 2]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]], [[0, 0], [0, 0], [0, 0], [0, 0]]]</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>[[0, 0], [0, 1], [0, 2], [0, 3]]</t>
+  </si>
+  <si>
+    <t>[[0, 0], [0, 0], [0, 1], [0, 2]]</t>
+  </si>
+  <si>
+    <t>[[0, 0], [0, 0], [0, 0], [0, 0]]</t>
+  </si>
+  <si>
+    <t>[[0, 0], [0, 0], [0, 0], [0, 1]]</t>
   </si>
 </sst>
 </file>
@@ -83,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,14 +192,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,32 +483,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="6" width="4.85546875" customWidth="1"/>
+    <col min="1" max="6" width="4.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="1"/>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -478,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -494,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -508,11 +552,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>0</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
@@ -522,9 +566,9 @@
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -541,42 +585,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -590,13 +634,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB56664-0B75-4CDF-A851-3E9A7FB4C2D2}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>11</v>
       </c>
@@ -613,7 +657,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -630,7 +674,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -647,7 +691,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -664,7 +708,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>7</v>
       </c>
@@ -681,7 +725,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -698,7 +742,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -715,7 +759,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -732,7 +776,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -743,19 +787,19 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>2</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -766,7 +810,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -783,16 +827,16 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>0</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -800,7 +844,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -816,39 +860,39 @@
       <c r="F13" s="1">
         <v>4</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="1">
         <v>5</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="1">
         <v>6</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="1">
         <v>7</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="1">
         <v>8</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="1">
         <v>9</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="1">
         <v>10</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -856,12 +900,196 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9215A50-F744-4EE1-A539-07EAB1ED11ED}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBAE232-842A-44D5-9CBC-A8152C18AA97}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="36.765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="b">
+        <f>(A3=A15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="b">
+        <f t="shared" ref="B4:B11" si="0">(A4=A16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>